<commit_message>
Actualización del repositorio - 23 de enero - Mac
</commit_message>
<xml_diff>
--- a/Bitacoras/NRC_163_Grupo_47/Parcial_02/Bitacora_Evaluacion_Continua_Parcial_02_NRC_163.xlsx
+++ b/Bitacoras/NRC_163_Grupo_47/Parcial_02/Bitacora_Evaluacion_Continua_Parcial_02_NRC_163.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Plan PU\Fisica_3\Bitacoras\NRC_163_Grupo_47\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavo/Documents/Cursos_UVM/PLAN_PU/UVM_PU_Fisica_3/Bitacoras/NRC_163_Grupo_47/Parcial_02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2D8352-EF5C-475A-B5CC-F00D31EDEE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1BF42B-9455-4B4D-A70D-BBD9F5FB73EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{7D2BE740-95B4-4318-9D40-57B175E37B29}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25640" windowHeight="14020" activeTab="1" xr2:uid="{7D2BE740-95B4-4318-9D40-57B175E37B29}"/>
   </bookViews>
   <sheets>
     <sheet name="Newton-Kepler" sheetId="1" r:id="rId1"/>
@@ -550,7 +550,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -565,6 +565,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -918,20 +921,20 @@
       <selection activeCell="M2" sqref="M2:M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -972,7 +975,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10185626</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20235058</v>
       </c>
@@ -1056,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20246860</v>
       </c>
@@ -1098,7 +1101,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>10187946</v>
       </c>
@@ -1140,7 +1143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20266381</v>
       </c>
@@ -1182,7 +1185,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>10187062</v>
       </c>
@@ -1224,7 +1227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20268481</v>
       </c>
@@ -1266,7 +1269,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20267076</v>
       </c>
@@ -1308,7 +1311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20255663</v>
       </c>
@@ -1350,7 +1353,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20256373</v>
       </c>
@@ -1392,7 +1395,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>20240735</v>
       </c>
@@ -1434,7 +1437,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10186997</v>
       </c>
@@ -1476,7 +1479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10187563</v>
       </c>
@@ -1518,7 +1521,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>10186666</v>
       </c>
@@ -1560,7 +1563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>20268087</v>
       </c>
@@ -1602,7 +1605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>20267318</v>
       </c>
@@ -1644,7 +1647,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>20265373</v>
       </c>
@@ -1686,7 +1689,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>10185884</v>
       </c>
@@ -1728,7 +1731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>10188303</v>
       </c>
@@ -1770,7 +1773,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20263060</v>
       </c>
@@ -1812,7 +1815,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20258138</v>
       </c>
@@ -1854,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20253903</v>
       </c>
@@ -1896,7 +1899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20264117</v>
       </c>
@@ -1938,7 +1941,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>10187574</v>
       </c>
@@ -1980,7 +1983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>10187795</v>
       </c>
@@ -2022,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>20263273</v>
       </c>
@@ -2076,21 +2079,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD29E299-235F-4B80-B5B3-5877D3CDF14E}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="11.42578125" style="1"/>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F1" s="1">
         <v>7</v>
       </c>
@@ -2114,7 +2116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2152,7 +2154,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10185626</v>
       </c>
@@ -2192,7 +2194,7 @@
         <v>9.891304347826086</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20235058</v>
       </c>
@@ -2232,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20246860</v>
       </c>
@@ -2272,7 +2274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>10187946</v>
       </c>
@@ -2312,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20266381</v>
       </c>
@@ -2352,7 +2354,7 @@
         <v>3.4782608695652173</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>10187062</v>
       </c>
@@ -2392,7 +2394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20268481</v>
       </c>
@@ -2432,11 +2434,11 @@
         <v>3.4782608695652173</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20267076</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>82</v>
       </c>
       <c r="C10" t="s">
@@ -2472,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20255663</v>
       </c>
@@ -2512,7 +2514,7 @@
         <v>2.3913043478260869</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>20256373</v>
       </c>
@@ -2546,7 +2548,7 @@
         <v>5.6521739130434776</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20240735</v>
       </c>
@@ -2586,7 +2588,7 @@
         <v>9.2391304347826093</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10186997</v>
       </c>
@@ -2626,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>10187563</v>
       </c>
@@ -2666,7 +2668,7 @@
         <v>5.8695652173913047</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>10186666</v>
       </c>
@@ -2706,7 +2708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>20268087</v>
       </c>
@@ -2746,7 +2748,7 @@
         <v>9.3478260869565215</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>20267318</v>
       </c>
@@ -2786,7 +2788,7 @@
         <v>8.2608695652173907</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>20265373</v>
       </c>
@@ -2826,7 +2828,7 @@
         <v>2.1739130434782608</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>10185884</v>
       </c>
@@ -2866,7 +2868,7 @@
         <v>9.0217391304347831</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>10188303</v>
       </c>
@@ -2897,7 +2899,7 @@
         <v>3.695652173913043</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20263060</v>
       </c>
@@ -2934,7 +2936,7 @@
         <v>5.8695652173913047</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20258138</v>
       </c>
@@ -2974,7 +2976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20253903</v>
       </c>
@@ -3014,7 +3016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>20264117</v>
       </c>
@@ -3054,7 +3056,7 @@
         <v>2.3913043478260869</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>10187574</v>
       </c>
@@ -3094,7 +3096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>10187795</v>
       </c>
@@ -3134,7 +3136,7 @@
         <v>1.3043478260869565</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>20263273</v>
       </c>
@@ -3169,13 +3171,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:L28" xr:uid="{FD29E299-235F-4B80-B5B3-5877D3CDF14E}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="ZAVALA ROMERO DIEGO"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:L28" xr:uid="{FD29E299-235F-4B80-B5B3-5877D3CDF14E}"/>
   <conditionalFormatting sqref="F3:G28">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
@@ -3198,20 +3194,20 @@
       <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="3.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="23" width="4.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="11.42578125" style="1"/>
-    <col min="28" max="28" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="23" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="11.5" style="1"/>
+    <col min="28" max="28" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -3296,7 +3292,7 @@
       </c>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3387,7 +3383,7 @@
       </c>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3478,7 +3474,7 @@
       </c>
       <c r="AD3" s="2"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3560,7 +3556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3652,7 +3648,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3749,7 +3745,7 @@
         <v>7.5549999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3847,7 +3843,7 @@
         <v>7.9328933333333342</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3934,7 +3930,7 @@
         <v>46.2</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4017,7 +4013,7 @@
         <v>9.4981000000000009</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4099,7 +4095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4182,7 +4178,7 @@
         <v>7.3331</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4265,7 +4261,7 @@
         <v>8.8331</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4348,7 +4344,7 @@
         <v>5.3331</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4431,7 +4427,7 @@
         <v>5.8331</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4513,7 +4509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4596,7 +4592,7 @@
         <v>6.8331</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4679,7 +4675,7 @@
         <v>7.8331</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4762,7 +4758,7 @@
         <v>4.3331</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4845,7 +4841,7 @@
         <v>6.3331</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4928,7 +4924,7 @@
         <v>8.4981000000000009</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -5011,7 +5007,7 @@
         <v>7.8331</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -5094,7 +5090,7 @@
         <v>4.3331</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -5177,7 +5173,7 @@
         <v>7.8331</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -5260,7 +5256,7 @@
         <v>7.8331</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -5343,7 +5339,7 @@
         <v>4.3331</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -5426,7 +5422,7 @@
         <v>8.3331</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -5519,19 +5515,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{081E9561-2928-41CB-8767-9EB69BD5826F}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B27"/>
+    <sheetView topLeftCell="B8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="30.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -5548,7 +5544,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5569,7 +5565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5590,7 +5586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5611,7 +5607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5632,7 +5628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5653,7 +5649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5674,7 +5670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5695,7 +5691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5716,7 +5712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5737,7 +5733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5758,7 +5754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5779,7 +5775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5800,7 +5796,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5821,7 +5817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5842,7 +5838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5863,7 +5859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5884,7 +5880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5905,7 +5901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5926,7 +5922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5947,7 +5943,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5968,7 +5964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5989,7 +5985,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -6010,7 +6006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -6031,7 +6027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -6052,7 +6048,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -6073,7 +6069,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>

</xml_diff>